<commit_message>
Começo dos cálculos do método SNA
Com algumas importações a mais feitas
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <t>VALORES CORRENTES</t>
   </si>
@@ -221,6 +221,30 @@
   </si>
   <si>
     <t>Índice RIB Pa</t>
+  </si>
+  <si>
+    <t>Consumo das Famílias - VN</t>
+  </si>
+  <si>
+    <t>Consumo do Governo - VN</t>
+  </si>
+  <si>
+    <t>PIB - VN</t>
+  </si>
+  <si>
+    <t>Formação Bruta de Capital Fixo - VN</t>
+  </si>
+  <si>
+    <t>Formação Bruta de Capital - VN</t>
+  </si>
+  <si>
+    <t>Exportação - VN</t>
+  </si>
+  <si>
+    <t>Importação - VN</t>
+  </si>
+  <si>
+    <t>Absorção Doméstica - VN</t>
   </si>
 </sst>
 </file>
@@ -1306,25 +1330,25 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="70425216"/>
-        <c:axId val="70431104"/>
+        <c:axId val="107821696"/>
+        <c:axId val="10859264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70425216"/>
+        <c:axId val="107821696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70431104"/>
+        <c:crossAx val="10859264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70431104"/>
+        <c:axId val="10859264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1332,7 +1356,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70425216"/>
+        <c:crossAx val="107821696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1342,7 +1366,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000036" footer="0.31496062000000036"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000041" footer="0.31496062000000041"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1368,7 +1392,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2273,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BK49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BH3" sqref="BH3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2443,28 +2467,28 @@
         <v>12</v>
       </c>
       <c r="J2" s="66" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="K2" s="67" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="L2" s="67" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="M2" s="67" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="N2" s="67" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="O2" s="67" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="P2" s="67" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="Q2" s="67" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="R2" s="68" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Atualização de arquivos fonte e resultados
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD1D086-E7AC-4DB9-87ED-5D8A65B8A970}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anual_1947-1989 (ref1987)" sheetId="4" r:id="rId1"/>
     <sheet name="Anual_1990-2000 (ref1985e2000)" sheetId="2" r:id="rId2"/>
-    <sheet name="Trimestral_1996-2018 (ref2010)" sheetId="3" r:id="rId3"/>
-    <sheet name="Anual_2000-2017 (ref2010)" sheetId="1" r:id="rId4"/>
+    <sheet name="Trimestral (ref2010)" sheetId="3" r:id="rId3"/>
+    <sheet name="Anual (ref2010)" sheetId="1" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -250,7 +256,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -1020,26 +1026,48 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal_quadro04B" xfId="4"/>
-    <cellStyle name="Separador de milhares" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal_quadro04B" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1054,6 +1082,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'[1]Anual_1947-1989 (ref1987)'!$A$5:$A$46</c:f>
@@ -1193,7 +1222,7 @@
             <c:numRef>
               <c:f>'[1]Anual_1947-1989 (ref1987)'!$BA$5:$BA$46</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>-3.2344234002100727E-3</c:v>
@@ -1324,12 +1353,21 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3E84-4FAE-9809-8DB61E85F00C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="107821696"/>
         <c:axId val="10859264"/>
       </c:barChart>
@@ -1338,23 +1376,30 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="10859264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="10859264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="107821696"/>
         <c:crosses val="autoZero"/>
@@ -1363,6 +1408,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1392,7 +1438,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1414,7 +1460,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Legenda"/>
@@ -2005,6 +2051,16 @@
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2013,7 +2069,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2051,9 +2107,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2085,9 +2141,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2119,9 +2193,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2294,11 +2386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="BA7" workbookViewId="0">
+      <selection activeCell="BK46" sqref="BK46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10424,19 +10516,19 @@
       </c>
       <c r="AK36" s="106">
         <f t="shared" si="22"/>
-        <v>2.3644900843900456</v>
+        <v>2.3644900843900452</v>
       </c>
       <c r="AL36" s="106">
         <f t="shared" si="23"/>
-        <v>1.2688214429288351</v>
+        <v>1.2688214429288349</v>
       </c>
       <c r="AM36" s="106">
         <f t="shared" si="24"/>
-        <v>1.293389286309772</v>
+        <v>1.2933892863097718</v>
       </c>
       <c r="AN36" s="106">
         <f t="shared" si="9"/>
-        <v>1.2044083496128029</v>
+        <v>1.2044083496128026</v>
       </c>
       <c r="AO36" s="105">
         <f t="shared" si="10"/>
@@ -11132,11 +11224,11 @@
       </c>
       <c r="AK39" s="106">
         <f t="shared" si="22"/>
-        <v>3.0707962302826473</v>
+        <v>3.0707962302826477</v>
       </c>
       <c r="AL39" s="106">
         <f t="shared" si="23"/>
-        <v>1.105085244954281</v>
+        <v>1.1050852449542812</v>
       </c>
       <c r="AM39" s="106">
         <f t="shared" si="24"/>
@@ -11144,7 +11236,7 @@
       </c>
       <c r="AN39" s="106">
         <f t="shared" si="9"/>
-        <v>1.3340488412569056</v>
+        <v>1.3340488412569058</v>
       </c>
       <c r="AO39" s="105">
         <f t="shared" si="10"/>
@@ -12536,19 +12628,19 @@
       </c>
       <c r="AK45" s="106">
         <f t="shared" si="22"/>
-        <v>11.314099640241388</v>
+        <v>11.314099640241389</v>
       </c>
       <c r="AL45" s="106">
         <f t="shared" si="23"/>
-        <v>0.60856098473946896</v>
+        <v>0.60856098473946907</v>
       </c>
       <c r="AM45" s="106">
         <f t="shared" si="24"/>
-        <v>0.81578579804733964</v>
+        <v>0.81578579804733975</v>
       </c>
       <c r="AN45" s="106">
         <f t="shared" si="9"/>
-        <v>0.79507268529110786</v>
+        <v>0.79507268529110797</v>
       </c>
       <c r="AO45" s="105">
         <f t="shared" si="10"/>
@@ -12776,19 +12868,19 @@
       </c>
       <c r="AK46" s="106">
         <f t="shared" si="22"/>
-        <v>24.784643002747195</v>
+        <v>24.784643002747199</v>
       </c>
       <c r="AL46" s="106">
         <f t="shared" si="23"/>
-        <v>1.4154483985098425</v>
+        <v>1.4154483985098427</v>
       </c>
       <c r="AM46" s="106">
         <f t="shared" si="24"/>
-        <v>0.8078893400065803</v>
+        <v>0.80788934000658041</v>
       </c>
       <c r="AN46" s="106">
         <f t="shared" si="9"/>
-        <v>0.86425023943624257</v>
+        <v>0.86425023943624268</v>
       </c>
       <c r="AO46" s="118">
         <f t="shared" si="10"/>
@@ -12921,11 +13013,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12957,7 +13049,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="18"/>
+      <c r="J1" s="2"/>
       <c r="K1" s="18" t="s">
         <v>14</v>
       </c>
@@ -12998,7 +13090,7 @@
       <c r="I2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="7" t="s">
@@ -13616,15 +13708,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="B3" sqref="B3:O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13735,7 +13828,6 @@
         <v>76119.962709045605</v>
       </c>
       <c r="H3" s="22">
-        <f t="shared" ref="H3:H25" si="0">SUM(C3:E3)</f>
         <v>885098.13842107123</v>
       </c>
       <c r="I3" s="22">
@@ -13783,7 +13875,6 @@
         <v>91329.724399258994</v>
       </c>
       <c r="H4" s="22">
-        <f t="shared" si="0"/>
         <v>989866.43511025887</v>
       </c>
       <c r="I4" s="22">
@@ -13831,7 +13922,6 @@
         <v>94302.031812068803</v>
       </c>
       <c r="H5" s="22">
-        <f t="shared" si="0"/>
         <v>1029967.6024543091</v>
       </c>
       <c r="I5" s="22">
@@ -13879,7 +13969,6 @@
         <v>124186.820162843</v>
       </c>
       <c r="H6" s="22">
-        <f t="shared" si="0"/>
         <v>1103798.8295971151</v>
       </c>
       <c r="I6" s="22">
@@ -13927,7 +14016,6 @@
         <v>149307.50751354202</v>
       </c>
       <c r="H7" s="22">
-        <f t="shared" si="0"/>
         <v>1219057.3629092062</v>
       </c>
       <c r="I7" s="22">
@@ -13975,7 +14063,6 @@
         <v>191634.18341005599</v>
       </c>
       <c r="H8" s="22">
-        <f t="shared" si="0"/>
         <v>1340348.1202247278</v>
       </c>
       <c r="I8" s="22">
@@ -14023,7 +14110,6 @@
         <v>199315.37083534192</v>
       </c>
       <c r="H9" s="22">
-        <f t="shared" si="0"/>
         <v>1483343.4777237489</v>
       </c>
       <c r="I9" s="22">
@@ -14071,7 +14157,6 @@
         <v>222639.51702602001</v>
       </c>
       <c r="H10" s="22">
-        <f t="shared" si="0"/>
         <v>1675463.5601042481</v>
       </c>
       <c r="I10" s="22">
@@ -14119,7 +14204,6 @@
         <v>257101.50118791108</v>
       </c>
       <c r="H11" s="22">
-        <f t="shared" si="0"/>
         <v>1879331.4213950306</v>
       </c>
       <c r="I11" s="22">
@@ -14167,7 +14251,6 @@
         <v>257061.583470515</v>
       </c>
       <c r="H12" s="22">
-        <f t="shared" si="0"/>
         <v>2093538.2318370175</v>
       </c>
       <c r="I12" s="22">
@@ -14215,7 +14298,6 @@
         <v>281119.76464654488</v>
       </c>
       <c r="H13" s="22">
-        <f t="shared" si="0"/>
         <v>2329622.2667676983</v>
       </c>
       <c r="I13" s="22">
@@ -14263,7 +14345,6 @@
         <v>325477.72680545301</v>
       </c>
       <c r="H14" s="22">
-        <f t="shared" si="0"/>
         <v>2633587.1050103479</v>
       </c>
       <c r="I14" s="22">
@@ -14305,13 +14386,12 @@
         <v>602845.57725732995</v>
       </c>
       <c r="F15" s="25">
-        <v>420880.76599999971</v>
+        <v>420880.76604035415</v>
       </c>
       <c r="G15" s="25">
-        <v>426775.9697999999</v>
+        <v>426775.9697693208</v>
       </c>
       <c r="H15" s="22">
-        <f t="shared" si="0"/>
         <v>3046223.6347877472</v>
       </c>
       <c r="I15" s="22">
@@ -14353,13 +14433,12 @@
         <v>636675.77898595296</v>
       </c>
       <c r="F16" s="25">
-        <v>361680.47040000034</v>
+        <v>361680.47039454698</v>
       </c>
       <c r="G16" s="25">
-        <v>375120.39620000089</v>
+        <v>375120.39618569904</v>
       </c>
       <c r="H16" s="22">
-        <f t="shared" si="0"/>
         <v>3356672.4818217042</v>
       </c>
       <c r="I16" s="22">
@@ -14401,35 +14480,34 @@
         <v>797945.99999999884</v>
       </c>
       <c r="F17" s="25">
-        <v>422220.00000000047</v>
+        <v>417270.00000000052</v>
       </c>
       <c r="G17" s="25">
-        <v>462671.99999999901</v>
+        <v>457722</v>
       </c>
       <c r="H17" s="22">
-        <f t="shared" si="0"/>
         <v>3877078.9999999981</v>
       </c>
       <c r="I17" s="22">
         <v>49219.999999999505</v>
       </c>
       <c r="J17" s="26">
-        <v>7.5282258303849492</v>
+        <v>7.5282258303847573</v>
       </c>
       <c r="K17" s="26">
-        <v>6.2293721263483315</v>
+        <v>6.2293721263484727</v>
       </c>
       <c r="L17" s="26">
-        <v>3.9206645935541129</v>
+        <v>3.9206645935543056</v>
       </c>
       <c r="M17" s="26">
-        <v>17.85392142269604</v>
+        <v>17.853921422696498</v>
       </c>
       <c r="N17" s="26">
-        <v>11.721721538659246</v>
+        <v>11.721721538658818</v>
       </c>
       <c r="O17" s="26">
-        <v>33.63902466469002</v>
+        <v>33.639024664689614</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -14449,35 +14527,34 @@
         <v>901926.99999999802</v>
       </c>
       <c r="F18" s="25">
-        <v>506895</v>
+        <v>501802</v>
       </c>
       <c r="G18" s="25">
-        <v>540565.99999999895</v>
+        <v>535473</v>
       </c>
       <c r="H18" s="22">
-        <f t="shared" si="0"/>
         <v>4356779.0000000009</v>
       </c>
       <c r="I18" s="22">
         <v>53273.999999994194</v>
       </c>
       <c r="J18" s="26">
-        <v>3.9744230794469759</v>
+        <v>3.9744230794471664</v>
       </c>
       <c r="K18" s="26">
-        <v>4.8184595372898098</v>
+        <v>4.8184595372894803</v>
       </c>
       <c r="L18" s="26">
-        <v>2.2042962734415417</v>
+        <v>2.2042962734413565</v>
       </c>
       <c r="M18" s="26">
-        <v>6.8340464141684709</v>
+        <v>6.8340464141682284</v>
       </c>
       <c r="N18" s="26">
-        <v>4.8119463786651995</v>
+        <v>4.8119463786650769</v>
       </c>
       <c r="O18" s="26">
-        <v>9.3932634782305726</v>
+        <v>9.3932634782305584</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -14497,35 +14574,34 @@
         <v>997459.99999999907</v>
       </c>
       <c r="F19" s="25">
-        <v>571875.00000000093</v>
+        <v>563474.00000000093</v>
       </c>
       <c r="G19" s="25">
-        <v>637317</v>
+        <v>628916</v>
       </c>
       <c r="H19" s="22">
-        <f t="shared" si="0"/>
         <v>4846474.0000000037</v>
       </c>
       <c r="I19" s="22">
         <v>33728.000000002801</v>
       </c>
       <c r="J19" s="26">
-        <v>1.9211759850945809</v>
+        <v>1.9211759850944119</v>
       </c>
       <c r="K19" s="26">
-        <v>3.4994506815110071</v>
+        <v>3.4994506815114335</v>
       </c>
       <c r="L19" s="26">
-        <v>2.2770054758775471</v>
+        <v>2.2770054758772393</v>
       </c>
       <c r="M19" s="26">
-        <v>0.7787769963642166</v>
+        <v>0.77877699636462638</v>
       </c>
       <c r="N19" s="26">
-        <v>0.70764162203225123</v>
+        <v>0.7076416220318984</v>
       </c>
       <c r="O19" s="26">
-        <v>1.1308517368831206</v>
+        <v>1.1308517368833524</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -14545,35 +14621,34 @@
         <v>1114944</v>
       </c>
       <c r="F20" s="25">
-        <v>626050.99999999895</v>
+        <v>620077.00000000093</v>
       </c>
       <c r="G20" s="25">
-        <v>748758</v>
+        <v>742784</v>
       </c>
       <c r="H20" s="22">
-        <f t="shared" si="0"/>
         <v>5412640.9999999972</v>
       </c>
       <c r="I20" s="22">
         <v>41685.000000002197</v>
       </c>
       <c r="J20" s="26">
-        <v>3.0048226702889202</v>
+        <v>3.0048226702888803</v>
       </c>
       <c r="K20" s="26">
-        <v>3.4710436906504771</v>
+        <v>3.4710436906500233</v>
       </c>
       <c r="L20" s="26">
-        <v>1.5101212759755178</v>
+        <v>1.5101212759755107</v>
       </c>
       <c r="M20" s="26">
-        <v>5.8272010907705507</v>
+        <v>5.8272010907704548</v>
       </c>
       <c r="N20" s="26">
-        <v>1.8302950819672592</v>
+        <v>1.8302950819671997</v>
       </c>
       <c r="O20" s="26">
-        <v>6.6696792961743911</v>
+        <v>6.6696792961742606</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -14581,10 +14656,10 @@
         <v>2014</v>
       </c>
       <c r="B21" s="25">
-        <v>5778953.0000000102</v>
+        <v>5778952.9999999991</v>
       </c>
       <c r="C21" s="25">
-        <v>3638404.0000000028</v>
+        <v>3638404.0000000061</v>
       </c>
       <c r="D21" s="25">
         <v>1106874</v>
@@ -14593,35 +14668,34 @@
         <v>1148452.9999999991</v>
       </c>
       <c r="F21" s="25">
-        <v>636374.99999999907</v>
+        <v>636374.99999999895</v>
       </c>
       <c r="G21" s="25">
         <v>790183.00000000093</v>
       </c>
       <c r="H21" s="22">
-        <f t="shared" si="0"/>
-        <v>5893731.0000000019</v>
+        <v>5893731.0000000047</v>
       </c>
       <c r="I21" s="22">
-        <v>39030.000000001499</v>
+        <v>39029.99999999709</v>
       </c>
       <c r="J21" s="26">
-        <v>0.50395574027313206</v>
+        <v>0.50395574027333101</v>
       </c>
       <c r="K21" s="26">
-        <v>2.2503192599611532</v>
+        <v>2.2503192599611368</v>
       </c>
       <c r="L21" s="26">
-        <v>0.81308480802171346</v>
+        <v>0.81308480802203331</v>
       </c>
       <c r="M21" s="26">
-        <v>-4.224068652775637</v>
+        <v>-4.22406865277532</v>
       </c>
       <c r="N21" s="26">
-        <v>-1.5696804253968577</v>
+        <v>-1.5696804253967958</v>
       </c>
       <c r="O21" s="26">
-        <v>-2.2718955924343476</v>
+        <v>-2.2718955924343875</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -14629,47 +14703,46 @@
         <v>2015</v>
       </c>
       <c r="B22" s="25">
-        <v>5995786.9999999898</v>
+        <v>5995786.9999999991</v>
       </c>
       <c r="C22" s="25">
-        <v>3835193.0000000042</v>
+        <v>3835192.9999999963</v>
       </c>
       <c r="D22" s="25">
-        <v>1185775.9999999991</v>
+        <v>1185776.0000000021</v>
       </c>
       <c r="E22" s="25">
-        <v>1069396.999999997</v>
+        <v>1069397.0000000009</v>
       </c>
       <c r="F22" s="25">
-        <v>773467.99999999988</v>
+        <v>773426.527</v>
       </c>
       <c r="G22" s="25">
-        <v>842614</v>
+        <v>844082.98</v>
       </c>
       <c r="H22" s="22">
-        <f t="shared" si="0"/>
-        <v>6090366.0000000009</v>
+        <v>6090365.9999999991</v>
       </c>
       <c r="I22" s="22">
-        <v>-25432.999999993397</v>
+        <v>-25432.999999989799</v>
       </c>
       <c r="J22" s="26">
-        <v>-3.5457633934727784</v>
+        <v>-3.5457633934727859</v>
       </c>
       <c r="K22" s="26">
-        <v>-3.2164927259314635</v>
+        <v>-3.2164927259317202</v>
       </c>
       <c r="L22" s="26">
-        <v>-1.4365682092091325</v>
+        <v>-1.4365682092091516</v>
       </c>
       <c r="M22" s="26">
-        <v>-13.946500205058465</v>
+        <v>-13.946500205058593</v>
       </c>
       <c r="N22" s="26">
-        <v>6.8195639363585192</v>
+        <v>6.8195639363581781</v>
       </c>
       <c r="O22" s="26">
-        <v>-14.190636852475723</v>
+        <v>-14.19063685247586</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -14677,47 +14750,46 @@
         <v>2016</v>
       </c>
       <c r="B23" s="25">
-        <v>6269328</v>
+        <v>6259227.7899210192</v>
       </c>
       <c r="C23" s="25">
-        <v>4028135.9999999981</v>
+        <v>4007330.4331000079</v>
       </c>
       <c r="D23" s="25">
-        <v>1277644.9999999988</v>
+        <v>1262801.9880000001</v>
       </c>
       <c r="E23" s="25">
-        <v>973271</v>
+        <v>1009175.689845003</v>
       </c>
       <c r="F23" s="25">
-        <v>781577.00000000012</v>
+        <v>782625.76199999999</v>
       </c>
       <c r="G23" s="25">
-        <v>756519.99999999895</v>
+        <v>759889.91500000004</v>
       </c>
       <c r="H23" s="22">
-        <f t="shared" si="0"/>
-        <v>6279051.9999999972</v>
+        <v>6279308.1109450115</v>
       </c>
       <c r="I23" s="22">
-        <v>-34781.000000002605</v>
+        <v>-46053.297024001993</v>
       </c>
       <c r="J23" s="26">
-        <v>-3.275916906320897</v>
+        <v>-3.3054543131704852</v>
       </c>
       <c r="K23" s="26">
-        <v>-3.8371993273870086</v>
+        <v>-3.8833769252290069</v>
       </c>
       <c r="L23" s="26">
-        <v>0.21100106596854129</v>
+        <v>0.2110010659687391</v>
       </c>
       <c r="M23" s="26">
-        <v>-12.129826434897495</v>
+        <v>-12.129826434897396</v>
       </c>
       <c r="N23" s="26">
-        <v>0.86312555916956413</v>
+        <v>0.86312555916975886</v>
       </c>
       <c r="O23" s="26">
-        <v>-10.342932825706841</v>
+        <v>-10.342932825706653</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -14725,47 +14797,46 @@
         <v>2017</v>
       </c>
       <c r="B24" s="25">
-        <v>6583319</v>
+        <v>6559940.2597514214</v>
       </c>
       <c r="C24" s="25">
-        <v>4245099.0000000102</v>
+        <v>4161219.81325013</v>
       </c>
       <c r="D24" s="25">
-        <v>1327758</v>
+        <v>1315135.6340000001</v>
       </c>
       <c r="E24" s="25">
-        <v>958779</v>
+        <v>1025615.2317722638</v>
       </c>
       <c r="F24" s="25">
-        <v>824434</v>
+        <v>824425.37100000004</v>
       </c>
       <c r="G24" s="25">
-        <v>777137.00000000093</v>
+        <v>757816.27600000007</v>
       </c>
       <c r="H24" s="22">
-        <f t="shared" si="0"/>
-        <v>6531636.0000000102</v>
+        <v>6501970.6790223932</v>
       </c>
       <c r="I24" s="22">
-        <v>4386.0000000001019</v>
+        <v>-8639.5142709723004</v>
       </c>
       <c r="J24" s="26">
-        <v>1.3228690539079935</v>
+        <v>1.0638612600035053</v>
       </c>
       <c r="K24" s="26">
-        <v>1.9779620151852306</v>
+        <v>1.3574273605176286</v>
       </c>
       <c r="L24" s="26">
-        <v>-0.67068708444074643</v>
+        <v>-0.86618692985959744</v>
       </c>
       <c r="M24" s="26">
-        <v>-2.5573555566745565</v>
+        <v>-2.4939572226026359</v>
       </c>
       <c r="N24" s="26">
-        <v>4.9087933754449642</v>
+        <v>5.2445300974822482</v>
       </c>
       <c r="O24" s="26">
-        <v>6.7169407285996297</v>
+        <v>4.987383677893642</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -14773,47 +14844,46 @@
         <v>2018</v>
       </c>
       <c r="B25" s="25">
-        <v>6889176.0835999902</v>
+        <v>6827585.9073859677</v>
       </c>
       <c r="C25" s="25">
-        <v>4457579.2630000096</v>
+        <v>4392357.3960216697</v>
       </c>
       <c r="D25" s="25">
-        <v>1383685.028999998</v>
+        <v>1346136.068</v>
       </c>
       <c r="E25" s="25">
-        <v>1049663.449</v>
+        <v>1080553.1380713417</v>
       </c>
       <c r="F25" s="25">
-        <v>1025777.6439999989</v>
+        <v>1010847.611</v>
       </c>
       <c r="G25" s="22">
-        <v>999487.36100000003</v>
+        <v>974754.91599999997</v>
       </c>
       <c r="H25" s="22">
-        <f t="shared" si="0"/>
-        <v>6890927.7410000078</v>
+        <v>6819046.6020930111</v>
       </c>
       <c r="I25" s="25">
-        <v>-28041.940399998704</v>
+        <v>-27553.389707043301</v>
       </c>
       <c r="J25" s="26">
-        <v>1.3172239968930022</v>
+        <v>1.1175791817495151</v>
       </c>
       <c r="K25" s="26">
-        <v>2.0550139348930019</v>
+        <v>1.8965327301248749</v>
       </c>
       <c r="L25" s="26">
-        <v>0.36043616381915555</v>
+        <v>1.7961063239900817E-2</v>
       </c>
       <c r="M25" s="26">
-        <v>3.9075078719912781</v>
+        <v>4.1307367763718528</v>
       </c>
       <c r="N25" s="26">
-        <v>3.9994379174076222</v>
+        <v>4.0545461998055474</v>
       </c>
       <c r="O25" s="26">
-        <v>8.3443002971163018</v>
+        <v>8.4949224197173638</v>
       </c>
     </row>
   </sheetData>
@@ -14822,11 +14892,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Atualização do 3º trimestre de 2021
Novos dados e resultados
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\rentainternabruta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\GitHub\rentainternabruta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB06976-BEDE-4C14-9C47-ACD49E086582}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C803A70-E75D-495E-95C3-40C1876E6476}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="795" windowWidth="14400" windowHeight="15750" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anual_1947-1989 (ref1987)" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <externalReferences>
     <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -11431,10 +11431,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11545,7 +11545,6 @@
         <v>76119.962709045605</v>
       </c>
       <c r="H3" s="22">
-        <f>SUM(C3:E3)</f>
         <v>885098.13842107123</v>
       </c>
       <c r="I3" s="22">
@@ -11593,7 +11592,6 @@
         <v>91329.724399258994</v>
       </c>
       <c r="H4" s="22">
-        <f t="shared" ref="H4:H27" si="0">SUM(C4:E4)</f>
         <v>989866.43511025887</v>
       </c>
       <c r="I4" s="22">
@@ -11641,7 +11639,6 @@
         <v>94302.031812068803</v>
       </c>
       <c r="H5" s="22">
-        <f t="shared" si="0"/>
         <v>1029967.6024543091</v>
       </c>
       <c r="I5" s="22">
@@ -11689,7 +11686,6 @@
         <v>124186.820162843</v>
       </c>
       <c r="H6" s="22">
-        <f t="shared" si="0"/>
         <v>1103798.8295971151</v>
       </c>
       <c r="I6" s="22">
@@ -11737,7 +11733,6 @@
         <v>149307.50751354202</v>
       </c>
       <c r="H7" s="22">
-        <f t="shared" si="0"/>
         <v>1219057.3629092062</v>
       </c>
       <c r="I7" s="22">
@@ -11785,7 +11780,6 @@
         <v>191634.18341005599</v>
       </c>
       <c r="H8" s="22">
-        <f t="shared" si="0"/>
         <v>1340348.1202247278</v>
       </c>
       <c r="I8" s="22">
@@ -11833,7 +11827,6 @@
         <v>199315.37083534192</v>
       </c>
       <c r="H9" s="22">
-        <f t="shared" si="0"/>
         <v>1483343.4777237489</v>
       </c>
       <c r="I9" s="22">
@@ -11881,7 +11874,6 @@
         <v>222639.51702602001</v>
       </c>
       <c r="H10" s="22">
-        <f t="shared" si="0"/>
         <v>1675463.5601042481</v>
       </c>
       <c r="I10" s="22">
@@ -11929,7 +11921,6 @@
         <v>257101.50118791108</v>
       </c>
       <c r="H11" s="22">
-        <f t="shared" si="0"/>
         <v>1879331.4213950306</v>
       </c>
       <c r="I11" s="22">
@@ -11977,7 +11968,6 @@
         <v>257061.583470515</v>
       </c>
       <c r="H12" s="22">
-        <f t="shared" si="0"/>
         <v>2093538.2318370175</v>
       </c>
       <c r="I12" s="22">
@@ -12025,7 +12015,6 @@
         <v>281119.76464654488</v>
       </c>
       <c r="H13" s="22">
-        <f t="shared" si="0"/>
         <v>2329622.2667676983</v>
       </c>
       <c r="I13" s="22">
@@ -12073,7 +12062,6 @@
         <v>325477.72680545301</v>
       </c>
       <c r="H14" s="22">
-        <f t="shared" si="0"/>
         <v>2633587.1050103479</v>
       </c>
       <c r="I14" s="22">
@@ -12121,7 +12109,6 @@
         <v>426775.9697999999</v>
       </c>
       <c r="H15" s="22">
-        <f t="shared" si="0"/>
         <v>3046223.6347877472</v>
       </c>
       <c r="I15" s="22">
@@ -12169,7 +12156,6 @@
         <v>375120.39620000089</v>
       </c>
       <c r="H16" s="22">
-        <f t="shared" si="0"/>
         <v>3356672.4818217042</v>
       </c>
       <c r="I16" s="22">
@@ -12199,47 +12185,46 @@
         <v>2010</v>
       </c>
       <c r="B17" s="25">
-        <v>3885847.0000000009</v>
+        <v>3885847.0002364516</v>
       </c>
       <c r="C17" s="25">
-        <v>2340166.9999999991</v>
+        <v>2340166.9989686897</v>
       </c>
       <c r="D17" s="25">
-        <v>738965.99999999895</v>
+        <v>738966.00021629594</v>
       </c>
       <c r="E17" s="25">
-        <v>797945.99999999907</v>
+        <v>797945.99977367104</v>
       </c>
       <c r="F17" s="25">
-        <v>422220.00000000029</v>
+        <v>422219.99999182345</v>
       </c>
       <c r="G17" s="25">
-        <v>462672.00000000099</v>
+        <v>462672.00000216858</v>
       </c>
       <c r="H17" s="22">
-        <f t="shared" si="0"/>
-        <v>3877078.9999999972</v>
+        <v>3877078.9989586566</v>
       </c>
       <c r="I17" s="22">
-        <v>49220.000000001099</v>
+        <v>49220.001288140302</v>
       </c>
       <c r="J17" s="26">
-        <v>7.5282258303846161</v>
+        <v>7.5282258217931108</v>
       </c>
       <c r="K17" s="26">
-        <v>6.2293721263483315</v>
+        <v>6.2293721234178534</v>
       </c>
       <c r="L17" s="26">
-        <v>3.9206645935543127</v>
+        <v>3.9206646429051251</v>
       </c>
       <c r="M17" s="26">
-        <v>17.85392142269593</v>
+        <v>17.853921357437951</v>
       </c>
       <c r="N17" s="26">
-        <v>11.721721538659091</v>
+        <v>11.721721514559192</v>
       </c>
       <c r="O17" s="26">
-        <v>33.639024664690268</v>
+        <v>33.639024641777723</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -12247,47 +12232,46 @@
         <v>2011</v>
       </c>
       <c r="B18" s="25">
-        <v>4376381.9999999907</v>
+        <v>4376381.9997261837</v>
       </c>
       <c r="C18" s="25">
-        <v>2637814.0000000028</v>
+        <v>2637813.9993392848</v>
       </c>
       <c r="D18" s="25">
-        <v>817038.00000000105</v>
+        <v>817037.99985351774</v>
       </c>
       <c r="E18" s="25">
-        <v>901926.99999999697</v>
+        <v>901926.99981083162</v>
       </c>
       <c r="F18" s="25">
-        <v>506895</v>
+        <v>506894.99988928612</v>
       </c>
       <c r="G18" s="25">
-        <v>540566</v>
+        <v>540566.00011584442</v>
       </c>
       <c r="H18" s="22">
-        <f t="shared" si="0"/>
-        <v>4356779.0000000009</v>
+        <v>4356778.9990036339</v>
       </c>
       <c r="I18" s="22">
-        <v>53273.999999998996</v>
+        <v>53274.000949107998</v>
       </c>
       <c r="J18" s="26">
-        <v>3.9744230794469537</v>
+        <v>3.9744230654152002</v>
       </c>
       <c r="K18" s="26">
-        <v>4.8184595372896544</v>
+        <v>4.8184595498840244</v>
       </c>
       <c r="L18" s="26">
-        <v>2.2042962734415417</v>
+        <v>2.2042962408155065</v>
       </c>
       <c r="M18" s="26">
-        <v>6.8340464141683599</v>
+        <v>6.8340464206406715</v>
       </c>
       <c r="N18" s="26">
-        <v>4.8119463786651773</v>
+        <v>4.8119463674623608</v>
       </c>
       <c r="O18" s="26">
-        <v>9.3932634782307964</v>
+        <v>9.3932634953357574</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -12295,47 +12279,46 @@
         <v>2012</v>
       </c>
       <c r="B19" s="25">
-        <v>4814759.9999999907</v>
+        <v>4814760.0000003316</v>
       </c>
       <c r="C19" s="25">
-        <v>2956833.9999999981</v>
+        <v>2956833.999595488</v>
       </c>
       <c r="D19" s="25">
-        <v>892180.00000000093</v>
+        <v>892179.9997161756</v>
       </c>
       <c r="E19" s="25">
-        <v>997459.99999999709</v>
+        <v>997460.00025951583</v>
       </c>
       <c r="F19" s="25">
-        <v>571875.00000000105</v>
+        <v>571875.00004342629</v>
       </c>
       <c r="G19" s="25">
-        <v>637317.00000000093</v>
+        <v>637317.00016246084</v>
       </c>
       <c r="H19" s="22">
-        <f t="shared" si="0"/>
-        <v>4846473.9999999963</v>
+        <v>4846473.99957118</v>
       </c>
       <c r="I19" s="22">
-        <v>33728.000000001099</v>
+        <v>33728.00054818661</v>
       </c>
       <c r="J19" s="26">
-        <v>1.9211759850947363</v>
+        <v>1.9211759930170214</v>
       </c>
       <c r="K19" s="26">
-        <v>3.4994506815110071</v>
+        <v>3.4994506869420183</v>
       </c>
       <c r="L19" s="26">
-        <v>2.2770054758774361</v>
+        <v>2.2770054602974765</v>
       </c>
       <c r="M19" s="26">
-        <v>0.77877699636434983</v>
+        <v>0.77877703109714425</v>
       </c>
       <c r="N19" s="26">
-        <v>0.70764162203216241</v>
+        <v>0.70764163070056174</v>
       </c>
       <c r="O19" s="26">
-        <v>1.1308517368834092</v>
+        <v>1.1308517342726976</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -12343,47 +12326,46 @@
         <v>2013</v>
       </c>
       <c r="B20" s="25">
-        <v>5331618.9999999898</v>
+        <v>5331618.9997678557</v>
       </c>
       <c r="C20" s="25">
-        <v>3290421.9999999963</v>
+        <v>3290421.9987369757</v>
       </c>
       <c r="D20" s="25">
-        <v>1007274.9999999991</v>
+        <v>1007275.0002494267</v>
       </c>
       <c r="E20" s="25">
-        <v>1114943.9999999981</v>
+        <v>1114944.0002428323</v>
       </c>
       <c r="F20" s="25">
-        <v>626051</v>
+        <v>626050.99995774194</v>
       </c>
       <c r="G20" s="25">
-        <v>748758</v>
+        <v>748758.0001349193</v>
       </c>
       <c r="H20" s="22">
-        <f t="shared" si="0"/>
-        <v>5412640.9999999935</v>
+        <v>5412640.9992292346</v>
       </c>
       <c r="I20" s="22">
-        <v>41685.000000005595</v>
+        <v>41685.000715798698</v>
       </c>
       <c r="J20" s="26">
-        <v>3.0048226702886316</v>
+        <v>3.0048226644272535</v>
       </c>
       <c r="K20" s="26">
-        <v>3.4710436906503217</v>
+        <v>3.4710436757441121</v>
       </c>
       <c r="L20" s="26">
-        <v>1.5101212759756732</v>
+        <v>1.5101213222501686</v>
       </c>
       <c r="M20" s="26">
-        <v>5.8272010907701732</v>
+        <v>5.827201090918277</v>
       </c>
       <c r="N20" s="26">
-        <v>1.830295081967348</v>
+        <v>1.8302950825010766</v>
       </c>
       <c r="O20" s="26">
-        <v>6.66967929617448</v>
+        <v>6.6696792999878518</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -12391,47 +12373,46 @@
         <v>2014</v>
       </c>
       <c r="B21" s="25">
-        <v>5778953</v>
+        <v>5778953.0004647188</v>
       </c>
       <c r="C21" s="25">
-        <v>3638404.0000000009</v>
+        <v>3638404.0000703488</v>
       </c>
       <c r="D21" s="25">
-        <v>1106873.9999999981</v>
+        <v>1106873.9997074394</v>
       </c>
       <c r="E21" s="25">
-        <v>1148452.9999999988</v>
+        <v>1148452.999930976</v>
       </c>
       <c r="F21" s="25">
-        <v>636375.00000000198</v>
+        <v>636375.00012536615</v>
       </c>
       <c r="G21" s="25">
-        <v>790183.00000000105</v>
+        <v>790183.00001008902</v>
       </c>
       <c r="H21" s="22">
-        <f t="shared" si="0"/>
-        <v>5893730.9999999981</v>
+        <v>5893730.9997087643</v>
       </c>
       <c r="I21" s="22">
-        <v>39030.000000003398</v>
+        <v>39030.000640677303</v>
       </c>
       <c r="J21" s="26">
-        <v>0.50395574027315426</v>
+        <v>0.50395575418937799</v>
       </c>
       <c r="K21" s="26">
-        <v>2.25031925996102</v>
+        <v>2.2503192809327777</v>
       </c>
       <c r="L21" s="26">
-        <v>0.81308480802153582</v>
+        <v>0.81308475783936629</v>
       </c>
       <c r="M21" s="26">
-        <v>-4.2240686527754034</v>
+        <v>-4.2240686681684352</v>
       </c>
       <c r="N21" s="26">
-        <v>-1.5696804253963137</v>
+        <v>-1.5696804123873309</v>
       </c>
       <c r="O21" s="26">
-        <v>-2.2718955924343254</v>
+        <v>-2.2718956166982496</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -12439,47 +12420,46 @@
         <v>2015</v>
       </c>
       <c r="B22" s="25">
-        <v>5995787</v>
+        <v>5995786.9998675892</v>
       </c>
       <c r="C22" s="25">
-        <v>3835192.9999999958</v>
+        <v>3835192.9998156349</v>
       </c>
       <c r="D22" s="25">
-        <v>1185776.0000000009</v>
+        <v>1185775.9996733265</v>
       </c>
       <c r="E22" s="25">
-        <v>1069396.999999997</v>
+        <v>1069396.9999630582</v>
       </c>
       <c r="F22" s="25">
-        <v>773468.00000000105</v>
+        <v>773468.00002799218</v>
       </c>
       <c r="G22" s="25">
-        <v>842614.00000000093</v>
+        <v>842613.99990513781</v>
       </c>
       <c r="H22" s="22">
-        <f t="shared" si="0"/>
-        <v>6090365.9999999935</v>
+        <v>6090365.9994520191</v>
       </c>
       <c r="I22" s="22">
-        <v>-25432.999999992295</v>
+        <v>-25432.9997072843</v>
       </c>
       <c r="J22" s="26">
-        <v>-3.5457633934728117</v>
+        <v>-3.5457634055206189</v>
       </c>
       <c r="K22" s="26">
-        <v>-3.21649272593163</v>
+        <v>-3.2164927280543432</v>
       </c>
       <c r="L22" s="26">
-        <v>-1.4365682092091436</v>
+        <v>-1.4365682016391323</v>
       </c>
       <c r="M22" s="26">
-        <v>-13.946500205058676</v>
+        <v>-13.946500214058222</v>
       </c>
       <c r="N22" s="26">
-        <v>6.8195639363584082</v>
+        <v>6.8195639403210828</v>
       </c>
       <c r="O22" s="26">
-        <v>-14.190636852475702</v>
+        <v>-14.190636857253281</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -12487,47 +12467,46 @@
         <v>2016</v>
       </c>
       <c r="B23" s="25">
-        <v>6269328</v>
+        <v>6269328.0001610899</v>
       </c>
       <c r="C23" s="25">
-        <v>4028136.0000000019</v>
+        <v>4028136.0009434354</v>
       </c>
       <c r="D23" s="25">
-        <v>1277645.0000000002</v>
+        <v>1277644.9999223293</v>
       </c>
       <c r="E23" s="25">
-        <v>973271</v>
+        <v>973270.99994744803</v>
       </c>
       <c r="F23" s="25">
-        <v>781577.00000000186</v>
+        <v>781576.9999849638</v>
       </c>
       <c r="G23" s="25">
-        <v>756520.00000000116</v>
+        <v>756520.00012595067</v>
       </c>
       <c r="H23" s="22">
-        <f t="shared" si="0"/>
-        <v>6279052.0000000019</v>
+        <v>6279052.0008132132</v>
       </c>
       <c r="I23" s="22">
-        <v>-34781.000000006396</v>
+        <v>-34781.000511135899</v>
       </c>
       <c r="J23" s="26">
-        <v>-3.2759169063210525</v>
+        <v>-3.2759169015248779</v>
       </c>
       <c r="K23" s="26">
-        <v>-3.8371993273870086</v>
+        <v>-3.8371992992595083</v>
       </c>
       <c r="L23" s="26">
-        <v>0.21100106596869672</v>
+        <v>0.21100107313554162</v>
       </c>
       <c r="M23" s="26">
-        <v>-12.129826434897417</v>
+        <v>-12.129826428435454</v>
       </c>
       <c r="N23" s="26">
-        <v>0.86312555916980838</v>
+        <v>0.86312555278482694</v>
       </c>
       <c r="O23" s="26">
-        <v>-10.342932825706708</v>
+        <v>-10.342932806323224</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -12535,47 +12514,46 @@
         <v>2017</v>
       </c>
       <c r="B24" s="25">
-        <v>6585478.9999999898</v>
+        <v>6585479.000297023</v>
       </c>
       <c r="C24" s="25">
-        <v>4247259</v>
+        <v>4247259.0003429661</v>
       </c>
       <c r="D24" s="25">
-        <v>1327757.999999996</v>
+        <v>1327757.9998302227</v>
       </c>
       <c r="E24" s="25">
-        <v>958778.9999999979</v>
+        <v>958778.99976894655</v>
       </c>
       <c r="F24" s="25">
-        <v>824434.00000000093</v>
+        <v>824434.00010073732</v>
       </c>
       <c r="G24" s="25">
-        <v>777137.00000000105</v>
+        <v>777136.9999805165</v>
       </c>
       <c r="H24" s="22">
-        <f t="shared" si="0"/>
-        <v>6533795.9999999944</v>
+        <v>6533795.9999421351</v>
       </c>
       <c r="I24" s="22">
-        <v>4385.9999999942993</v>
+        <v>4386.0002346676993</v>
       </c>
       <c r="J24" s="26">
-        <v>1.3228690539081489</v>
+        <v>1.3228690554852651</v>
       </c>
       <c r="K24" s="26">
-        <v>1.977962015184942</v>
+        <v>1.9779619958762984</v>
       </c>
       <c r="L24" s="26">
-        <v>-0.67068708444055769</v>
+        <v>-0.67068708922164433</v>
       </c>
       <c r="M24" s="26">
-        <v>-2.557355556674934</v>
+        <v>-2.5573555715094343</v>
       </c>
       <c r="N24" s="26">
-        <v>4.908793375444831</v>
+        <v>4.9087933820289864</v>
       </c>
       <c r="O24" s="26">
-        <v>6.7169407285997629</v>
+        <v>6.7169407145706295</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -12583,47 +12561,46 @@
         <v>2018</v>
       </c>
       <c r="B25" s="25">
-        <v>7004141</v>
+        <v>7004140.9998326944</v>
       </c>
       <c r="C25" s="25">
-        <v>4525801</v>
+        <v>4525800.9997553313</v>
       </c>
       <c r="D25" s="25">
-        <v>1393480.0000000012</v>
+        <v>1393480.0002171176</v>
       </c>
       <c r="E25" s="25">
-        <v>1057408.9999999991</v>
+        <v>1057409.0003329839</v>
       </c>
       <c r="F25" s="25">
-        <v>1025056.000000001</v>
+        <v>1025055.9999773456</v>
       </c>
       <c r="G25" s="22">
-        <v>997474.00000000093</v>
+        <v>997473.99975615717</v>
       </c>
       <c r="H25" s="22">
-        <f t="shared" si="0"/>
-        <v>6976690</v>
+        <v>6976690.0003054328</v>
       </c>
       <c r="I25" s="25">
-        <v>-131.00000000259024</v>
+        <v>-131.00069392610021</v>
       </c>
       <c r="J25" s="26">
-        <v>1.7836667613697621</v>
+        <v>1.7836667548653873</v>
       </c>
       <c r="K25" s="26">
-        <v>2.3659023384260625</v>
+        <v>2.3659023264338774</v>
       </c>
       <c r="L25" s="26">
-        <v>0.7868903821326878</v>
+        <v>0.78689042021597988</v>
       </c>
       <c r="M25" s="26">
-        <v>5.2317583092663877</v>
+        <v>5.2317583519554622</v>
       </c>
       <c r="N25" s="26">
-        <v>4.0530836913568846</v>
+        <v>4.0530836800943826</v>
       </c>
       <c r="O25" s="26">
-        <v>7.7427789437383598</v>
+        <v>7.7427789280271053</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -12631,47 +12608,46 @@
         <v>2019</v>
       </c>
       <c r="B26" s="25">
-        <v>7407023.5734999897</v>
+        <v>7389131.0005329112</v>
       </c>
       <c r="C26" s="25">
-        <v>4797117.8599999994</v>
+        <v>4813579.0001044171</v>
       </c>
       <c r="D26" s="25">
-        <v>1487164.1589999979</v>
+        <v>1476612.9994743918</v>
       </c>
       <c r="E26" s="25">
-        <v>1134199.929999999</v>
+        <v>1143184.9998809427</v>
       </c>
       <c r="F26" s="25">
-        <v>1044787.498000003</v>
+        <v>1043561.0000080449</v>
       </c>
       <c r="G26" s="22">
-        <v>1062950.486999999</v>
+        <v>1091178.0002049124</v>
       </c>
       <c r="H26" s="22">
-        <f t="shared" si="0"/>
-        <v>7418481.9489999963</v>
+        <v>7433376.9994597519</v>
       </c>
       <c r="I26" s="25">
-        <v>6704.6134999889036</v>
+        <v>3371.0012700264051</v>
       </c>
       <c r="J26" s="26">
-        <v>1.4111529850701077</v>
+        <v>1.220777831119757</v>
       </c>
       <c r="K26" s="26">
-        <v>2.1913704115581467</v>
+        <v>2.5953417052556382</v>
       </c>
       <c r="L26" s="26">
-        <v>-0.44532415248176305</v>
+        <v>-0.48619289369814522</v>
       </c>
       <c r="M26" s="26">
-        <v>3.3641057528354557</v>
+        <v>4.026067460927063</v>
       </c>
       <c r="N26" s="26">
-        <v>-2.3822259466798057</v>
+        <v>-2.5614210432762352</v>
       </c>
       <c r="O26" s="26">
-        <v>1.1256862835523629</v>
+        <v>1.3325660945815665</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -12679,47 +12655,93 @@
         <v>2020</v>
       </c>
       <c r="B27" s="25">
-        <v>7447858.2502464028</v>
+        <v>7467616.3893748512</v>
       </c>
       <c r="C27" s="25">
-        <v>4670909.6344771497</v>
+        <v>4696415.7282221969</v>
       </c>
       <c r="D27" s="25">
-        <v>1526283.48</v>
+        <v>1529313.1438056459</v>
       </c>
       <c r="E27" s="25">
-        <v>1223733.42179369</v>
+        <v>1240167.2452896901</v>
       </c>
       <c r="F27" s="25">
-        <v>1256517.3539999998</v>
+        <v>1254191.2828873987</v>
       </c>
       <c r="G27" s="22">
-        <v>1153184.7409999999</v>
+        <v>1201941.5090257295</v>
       </c>
       <c r="H27" s="22">
-        <f t="shared" si="0"/>
-        <v>7420926.5362708401</v>
+        <v>7465896.1173175322</v>
       </c>
       <c r="I27" s="25">
-        <v>-76400.899024436512</v>
+        <v>-50529.501804351305</v>
       </c>
       <c r="J27" s="26">
-        <v>-4.0590482726728494</v>
+        <v>-3.8786763342577357</v>
       </c>
       <c r="K27" s="26">
-        <v>-5.4544771520292805</v>
+        <v>-5.4452959905676561</v>
       </c>
       <c r="L27" s="26">
-        <v>-4.6800480349660001</v>
+        <v>-4.501546224951869</v>
       </c>
       <c r="M27" s="26">
-        <v>-0.77668563716366545</v>
+        <v>-0.52068490972366765</v>
       </c>
       <c r="N27" s="26">
-        <v>-1.7560833217400318</v>
+        <v>-1.842904729380046</v>
       </c>
       <c r="O27" s="26">
-        <v>-9.9520456779280906</v>
+        <v>-9.8406184954688332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="24">
+        <v>2021</v>
+      </c>
+      <c r="B28" s="25">
+        <v>6421742.1517525651</v>
+      </c>
+      <c r="C28" s="25">
+        <v>3839348.6701671979</v>
+      </c>
+      <c r="D28" s="25">
+        <v>1172913.9310000001</v>
+      </c>
+      <c r="E28" s="25">
+        <v>1235112.3634788422</v>
+      </c>
+      <c r="F28" s="25">
+        <v>1304454.399</v>
+      </c>
+      <c r="G28" s="22">
+        <v>1192506.061</v>
+      </c>
+      <c r="H28" s="22">
+        <v>6247374.9646460405</v>
+      </c>
+      <c r="I28" s="25">
+        <v>62418.849106525537</v>
+      </c>
+      <c r="J28" s="26">
+        <v>3.9400880865863686</v>
+      </c>
+      <c r="K28" s="26">
+        <v>2.1343772426789753</v>
+      </c>
+      <c r="L28" s="26">
+        <v>0.4091159576386838</v>
+      </c>
+      <c r="M28" s="26">
+        <v>20.240298742517361</v>
+      </c>
+      <c r="N28" s="26">
+        <v>3.8369814788677736</v>
+      </c>
+      <c r="O28" s="26">
+        <v>10.276774714681913</v>
       </c>
     </row>
   </sheetData>
@@ -12730,10 +12752,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12871,7 +12893,6 @@
         <v>-149307.50751354199</v>
       </c>
       <c r="J3" s="10">
-        <f t="shared" ref="J3:J21" si="0">SUM(C3:G3)</f>
         <v>1226235.5026320326</v>
       </c>
       <c r="K3" s="11"/>
@@ -12913,7 +12934,6 @@
         <v>-191634.18341005599</v>
       </c>
       <c r="J4" s="10">
-        <f t="shared" si="0"/>
         <v>1344608.191604831</v>
       </c>
       <c r="K4" s="13">
@@ -12941,7 +12961,6 @@
         <v>-154281.54206721316</v>
       </c>
       <c r="S4" s="15">
-        <f>SUM(L4:P4)</f>
         <v>1236599.2868735667</v>
       </c>
     </row>
@@ -12974,7 +12993,6 @@
         <v>-199315.37083534204</v>
       </c>
       <c r="J5" s="10">
-        <f t="shared" si="0"/>
         <v>1476239.4116588703</v>
       </c>
       <c r="K5" s="13">
@@ -13002,7 +13020,6 @@
         <v>-166132.90713136178</v>
       </c>
       <c r="S5" s="15">
-        <f t="shared" ref="S5:S21" si="1">SUM(L5:P5)</f>
         <v>1348739.9413477066</v>
       </c>
     </row>
@@ -13035,7 +13052,6 @@
         <v>-222639.51702601978</v>
       </c>
       <c r="J6" s="10">
-        <f t="shared" si="0"/>
         <v>1679791.5795973029</v>
       </c>
       <c r="K6" s="13">
@@ -13063,7 +13079,6 @@
         <v>-198351.68658387841</v>
       </c>
       <c r="S6" s="15">
-        <f t="shared" si="1"/>
         <v>1468921.5208193646</v>
       </c>
     </row>
@@ -13096,7 +13111,6 @@
         <v>-257101.50118791065</v>
       </c>
       <c r="J7" s="10">
-        <f t="shared" si="0"/>
         <v>1890927.8674182508</v>
       </c>
       <c r="K7" s="13">
@@ -13124,7 +13138,6 @@
         <v>-245713.97731488367</v>
       </c>
       <c r="S7" s="15">
-        <f t="shared" si="1"/>
         <v>1764071.9988808399</v>
       </c>
     </row>
@@ -13157,7 +13170,6 @@
         <v>-257061.58347051512</v>
       </c>
       <c r="J8" s="10">
-        <f t="shared" si="0"/>
         <v>2096765.8911171195</v>
       </c>
       <c r="K8" s="13">
@@ -13185,7 +13197,6 @@
         <v>-276284.70035073918</v>
       </c>
       <c r="S8" s="15">
-        <f t="shared" si="1"/>
         <v>1941560.9713275023</v>
       </c>
     </row>
@@ -13218,7 +13229,6 @@
         <v>-281119.76464654546</v>
       </c>
       <c r="J9" s="10">
-        <f t="shared" si="0"/>
         <v>2344227.7337713647</v>
       </c>
       <c r="K9" s="13">
@@ -13246,7 +13256,6 @@
         <v>-302722.36463419098</v>
       </c>
       <c r="S9" s="15">
-        <f t="shared" si="1"/>
         <v>2212418.8942733821</v>
       </c>
     </row>
@@ -13279,7 +13288,6 @@
         <v>-325477.72680545284</v>
       </c>
       <c r="J10" s="10">
-        <f t="shared" si="0"/>
         <v>2683192.8583180755</v>
       </c>
       <c r="K10" s="13">
@@ -13307,7 +13315,6 @@
         <v>-336100.03997604398</v>
       </c>
       <c r="S10" s="15">
-        <f t="shared" si="1"/>
         <v>2524068.0706767226</v>
       </c>
     </row>
@@ -13340,7 +13347,6 @@
         <v>-426775.96976932103</v>
       </c>
       <c r="J11" s="10">
-        <f t="shared" si="0"/>
         <v>3115698.2927752519</v>
       </c>
       <c r="K11" s="13">
@@ -13368,7 +13374,6 @@
         <v>-380892.62158459</v>
       </c>
       <c r="S11" s="15">
-        <f t="shared" si="1"/>
         <v>2875699.5335032512</v>
       </c>
     </row>
@@ -13401,7 +13406,6 @@
         <v>-375120.39618569863</v>
       </c>
       <c r="J12" s="10">
-        <f t="shared" si="0"/>
         <v>3346479.2812135681</v>
       </c>
       <c r="K12" s="13">
@@ -13429,7 +13433,6 @@
         <v>-394332.59932668612</v>
       </c>
       <c r="S12" s="15">
-        <f t="shared" si="1"/>
         <v>3118261.5410387437</v>
       </c>
     </row>
@@ -13462,7 +13465,6 @@
         <v>-462672</v>
       </c>
       <c r="J13" s="10">
-        <f t="shared" si="0"/>
         <v>3926299</v>
       </c>
       <c r="K13" s="13">
@@ -13490,7 +13492,6 @@
         <v>-501307.23883000016</v>
       </c>
       <c r="S13" s="15">
-        <f t="shared" si="1"/>
         <v>3681189.6755470159</v>
       </c>
     </row>
@@ -13523,7 +13524,6 @@
         <v>-540566</v>
       </c>
       <c r="J14" s="10">
-        <f t="shared" si="0"/>
         <v>4410053</v>
       </c>
       <c r="K14" s="13">
@@ -13551,7 +13551,6 @@
         <v>-506132</v>
       </c>
       <c r="S14" s="15">
-        <f t="shared" si="1"/>
         <v>4103882</v>
       </c>
     </row>
@@ -13584,7 +13583,6 @@
         <v>-637317</v>
       </c>
       <c r="J15" s="10">
-        <f t="shared" si="0"/>
         <v>4880202</v>
       </c>
       <c r="K15" s="13">
@@ -13612,7 +13610,6 @@
         <v>-546679</v>
       </c>
       <c r="S15" s="15">
-        <f t="shared" si="1"/>
         <v>4496657</v>
       </c>
     </row>
@@ -13645,7 +13642,6 @@
         <v>-748758</v>
       </c>
       <c r="J16" s="10">
-        <f t="shared" si="0"/>
         <v>5454326</v>
       </c>
       <c r="K16" s="13">
@@ -13673,7 +13669,6 @@
         <v>-679824</v>
       </c>
       <c r="S16" s="15">
-        <f t="shared" si="1"/>
         <v>5056917</v>
       </c>
     </row>
@@ -13706,7 +13701,6 @@
         <v>-790183</v>
       </c>
       <c r="J17" s="10">
-        <f t="shared" si="0"/>
         <v>5932761</v>
       </c>
       <c r="K17" s="13">
@@ -13734,7 +13728,6 @@
         <v>-731747</v>
       </c>
       <c r="S17" s="15">
-        <f t="shared" si="1"/>
         <v>5474011</v>
       </c>
     </row>
@@ -13767,7 +13760,6 @@
         <v>-842614</v>
       </c>
       <c r="J18" s="10">
-        <f t="shared" si="0"/>
         <v>6064933</v>
       </c>
       <c r="K18" s="13">
@@ -13795,7 +13787,6 @@
         <v>-678051</v>
       </c>
       <c r="S18" s="15">
-        <f t="shared" si="1"/>
         <v>5572323</v>
       </c>
     </row>
@@ -13828,7 +13819,6 @@
         <v>-756520</v>
       </c>
       <c r="J19" s="10">
-        <f t="shared" si="0"/>
         <v>6244271</v>
       </c>
       <c r="K19" s="13">
@@ -13856,7 +13846,6 @@
         <v>-755463</v>
       </c>
       <c r="S19" s="15">
-        <f t="shared" si="1"/>
         <v>5774689</v>
       </c>
     </row>
@@ -13889,7 +13878,6 @@
         <v>-777137</v>
       </c>
       <c r="J20" s="10">
-        <f t="shared" si="0"/>
         <v>6538182</v>
       </c>
       <c r="K20" s="13">
@@ -13917,7 +13905,6 @@
         <v>-807335</v>
       </c>
       <c r="S20" s="15">
-        <f t="shared" si="1"/>
         <v>6339655</v>
       </c>
     </row>
@@ -13950,7 +13937,6 @@
         <v>-997474</v>
       </c>
       <c r="J21" s="10">
-        <f t="shared" si="0"/>
         <v>6976559</v>
       </c>
       <c r="K21" s="13">
@@ -13978,8 +13964,66 @@
         <v>-837309</v>
       </c>
       <c r="S21" s="15">
-        <f t="shared" si="1"/>
         <v>6682402</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B22" s="9">
+        <v>7389131</v>
+      </c>
+      <c r="C22" s="9">
+        <v>4705528</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1476613</v>
+      </c>
+      <c r="E22" s="9">
+        <v>108051</v>
+      </c>
+      <c r="F22" s="9">
+        <v>1143185</v>
+      </c>
+      <c r="G22" s="9">
+        <v>3371</v>
+      </c>
+      <c r="H22" s="9">
+        <v>1043561</v>
+      </c>
+      <c r="I22" s="9">
+        <v>-1091178</v>
+      </c>
+      <c r="J22" s="10">
+        <v>7436748</v>
+      </c>
+      <c r="K22" s="13">
+        <v>7089646</v>
+      </c>
+      <c r="L22" s="14">
+        <v>4539601</v>
+      </c>
+      <c r="M22" s="14">
+        <v>1386705</v>
+      </c>
+      <c r="N22" s="14">
+        <v>103660</v>
+      </c>
+      <c r="O22" s="14">
+        <v>1099981</v>
+      </c>
+      <c r="P22" s="14">
+        <v>-28335</v>
+      </c>
+      <c r="Q22" s="15">
+        <v>998800</v>
+      </c>
+      <c r="R22" s="14">
+        <v>-1010766</v>
+      </c>
+      <c r="S22" s="15">
+        <v>7101612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>